<commit_message>
Atualização do script, adicionando funcionalidade de tratamento de dados da descrição do chamado, inserção de log, e verificação se campos então preenchidos corretamente.
</commit_message>
<xml_diff>
--- a/chamados.xlsx
+++ b/chamados.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\kali-linux\home\felipesouza\Documents\projetoChmadosSua\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\kali-linux\home\felipe\Documents\projetoChmadosSua\automarizacaoSua\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5613A4A-A12E-4940-9452-04B97A64C6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE725FA-4DD2-4A4F-BFF1-6ACF610CC56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00F37107-7D40-4ADB-921F-DDFA62B1AA1C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00F37107-7D40-4ADB-921F-DDFA62B1AA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
-    <sheet name="ATRIBUIDO" sheetId="4" r:id="rId2"/>
-    <sheet name="TITULO" sheetId="3" r:id="rId3"/>
-    <sheet name="LOCALIZAÇÃO" sheetId="2" r:id="rId4"/>
+    <sheet name="TITULO" sheetId="3" r:id="rId2"/>
+    <sheet name="CATEGORIA" sheetId="5" r:id="rId3"/>
+    <sheet name="ATRIBUIDO" sheetId="4" r:id="rId4"/>
+    <sheet name="LOCALIZAÇÃO" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MAIN!$A$1:$F$77</definedName>
@@ -41,8 +42,70 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Felipe Souza</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F6AE4DFF-62CF-4F58-976F-53C2911121E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="28"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>"Use palavras-chave como: Problema:, Unidade:, Patrimônio:, Modelo:, Local: para organizar a descrição. Use apenas as que forem necessárias."</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{C71415F2-CD59-4CEE-9327-4F49795F1FAE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="26"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hora deve serguir esse padrão: 25/06/2025  13:00:00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{B89011F1-16F2-479B-830C-046990E0E26A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Felipe Souza:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="221">
   <si>
     <t>TITULO</t>
   </si>
@@ -695,7 +758,16 @@
     <t>TROCA DE HD POR SSD</t>
   </si>
   <si>
-    <t>Problema: Troca de HD por SSD / Unidade: Francisco Eduardo de Paiva</t>
+    <t>MUDANÇA DE LOCAL DO COMPUTADOR</t>
+  </si>
+  <si>
+    <t>SUPORTE SEI</t>
+  </si>
+  <si>
+    <t>Problema: Suporte SEI Unidade: Mariano Gonzaga</t>
+  </si>
+  <si>
+    <t>25/06/2025  13:45:00</t>
   </si>
 </sst>
 </file>
@@ -705,7 +777,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -751,8 +823,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -774,6 +886,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1087,14 +1211,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1110,6 +1234,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1428,25 +1556,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D6CDD5-46C2-41B8-B947-C28F11FD0B44}">
-  <dimension ref="A1:K9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D6CDD5-46C2-41B8-B947-C28F11FD0B44}">
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="43.88671875" customWidth="1"/>
+    <col min="2" max="2" width="36.5546875" customWidth="1"/>
+    <col min="3" max="3" width="49.21875" customWidth="1"/>
+    <col min="4" max="4" width="64.6640625" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="144" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="7" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="39" x14ac:dyDescent="0.75">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -1462,50 +1590,1219 @@
       <c r="E1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="48" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="50">
-        <v>45833.472222222219</v>
-      </c>
-      <c r="D2" s="49" t="s">
+    <row r="2" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A2" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>220</v>
+      </c>
+      <c r="D2" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="51" t="str">
+      <c r="G2" s="52" t="str">
         <f>IF(F2&lt;&gt;"",VLOOKUP(F2,LOCALIZAÇÃO!A3:D79,4,FALSE),"")</f>
         <v>Diretoria de Assistência a Saúde &gt; Departamento de Unidade Básica de Saúde &gt; Unidades de Saúde da Família</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A3" s="49"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="52" t="str">
+        <f>IF(F3&lt;&gt;"",VLOOKUP(F3,LOCALIZAÇÃO!A4:D80,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="52" t="str">
+        <f>IF(F4&lt;&gt;"",VLOOKUP(F4,LOCALIZAÇÃO!A5:D81,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A5" s="49"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="52" t="str">
+        <f>IF(F5&lt;&gt;"",VLOOKUP(F5,LOCALIZAÇÃO!A6:D82,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A6" s="49"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="52" t="str">
+        <f>IF(F6&lt;&gt;"",VLOOKUP(F6,LOCALIZAÇÃO!A7:D83,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A7" s="49"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="52" t="str">
+        <f>IF(F7&lt;&gt;"",VLOOKUP(F7,LOCALIZAÇÃO!A8:D84,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="52" t="str">
+        <f>IF(F8&lt;&gt;"",VLOOKUP(F8,LOCALIZAÇÃO!A9:D85,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A9" s="49"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="52" t="str">
+        <f>IF(F9&lt;&gt;"",VLOOKUP(F9,LOCALIZAÇÃO!A10:D86,4,FALSE),"")</f>
+        <v/>
+      </c>
       <c r="K9" s="1"/>
     </row>
+    <row r="10" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A10" s="49"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="52" t="str">
+        <f>IF(F10&lt;&gt;"",VLOOKUP(F10,LOCALIZAÇÃO!A11:D87,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A11" s="49"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="52" t="str">
+        <f>IF(F11&lt;&gt;"",VLOOKUP(F11,LOCALIZAÇÃO!A12:D88,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="52" t="str">
+        <f>IF(F12&lt;&gt;"",VLOOKUP(F12,LOCALIZAÇÃO!A13:D89,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A13" s="49"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="52" t="str">
+        <f>IF(F13&lt;&gt;"",VLOOKUP(F13,LOCALIZAÇÃO!A14:D90,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A14" s="49"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="52" t="str">
+        <f>IF(F14&lt;&gt;"",VLOOKUP(F14,LOCALIZAÇÃO!A15:D91,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A15" s="49"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="52" t="str">
+        <f>IF(F15&lt;&gt;"",VLOOKUP(F15,LOCALIZAÇÃO!A16:D92,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="52" t="str">
+        <f>IF(F16&lt;&gt;"",VLOOKUP(F16,LOCALIZAÇÃO!A17:D93,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A17" s="49"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="52" t="str">
+        <f>IF(F17&lt;&gt;"",VLOOKUP(F17,LOCALIZAÇÃO!A18:D94,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A18" s="49"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="52" t="str">
+        <f>IF(F18&lt;&gt;"",VLOOKUP(F18,LOCALIZAÇÃO!A19:D95,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="52" t="str">
+        <f>IF(F19&lt;&gt;"",VLOOKUP(F19,LOCALIZAÇÃO!A20:D96,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="52" t="str">
+        <f>IF(F20&lt;&gt;"",VLOOKUP(F20,LOCALIZAÇÃO!A21:D97,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A21" s="49"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="52" t="str">
+        <f>IF(F21&lt;&gt;"",VLOOKUP(F21,LOCALIZAÇÃO!A22:D98,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A22" s="49"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="52" t="str">
+        <f>IF(F22&lt;&gt;"",VLOOKUP(F22,LOCALIZAÇÃO!A23:D99,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="52" t="str">
+        <f>IF(F23&lt;&gt;"",VLOOKUP(F23,LOCALIZAÇÃO!A24:D100,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A24" s="49"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="52" t="str">
+        <f>IF(F24&lt;&gt;"",VLOOKUP(F24,LOCALIZAÇÃO!A25:D101,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="52" t="str">
+        <f>IF(F25&lt;&gt;"",VLOOKUP(F25,LOCALIZAÇÃO!A26:D102,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A26" s="49"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="52" t="str">
+        <f>IF(F26&lt;&gt;"",VLOOKUP(F26,LOCALIZAÇÃO!A27:D103,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A27" s="49"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="52" t="str">
+        <f>IF(F27&lt;&gt;"",VLOOKUP(F27,LOCALIZAÇÃO!A28:D104,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A28" s="49"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="52" t="str">
+        <f>IF(F28&lt;&gt;"",VLOOKUP(F28,LOCALIZAÇÃO!A29:D105,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A29" s="49"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="52" t="str">
+        <f>IF(F29&lt;&gt;"",VLOOKUP(F29,LOCALIZAÇÃO!A30:D106,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A30" s="49"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="52" t="str">
+        <f>IF(F30&lt;&gt;"",VLOOKUP(F30,LOCALIZAÇÃO!A31:D107,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A31" s="49"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="52" t="str">
+        <f>IF(F31&lt;&gt;"",VLOOKUP(F31,LOCALIZAÇÃO!A32:D108,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A32" s="49"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="52" t="str">
+        <f>IF(F32&lt;&gt;"",VLOOKUP(F32,LOCALIZAÇÃO!A33:D109,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A33" s="49"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="52" t="str">
+        <f>IF(F33&lt;&gt;"",VLOOKUP(F33,LOCALIZAÇÃO!A34:D110,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A34" s="49"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="52" t="str">
+        <f>IF(F34&lt;&gt;"",VLOOKUP(F34,LOCALIZAÇÃO!A35:D111,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A35" s="49"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="52" t="str">
+        <f>IF(F35&lt;&gt;"",VLOOKUP(F35,LOCALIZAÇÃO!A36:D112,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A36" s="49"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="52" t="str">
+        <f>IF(F36&lt;&gt;"",VLOOKUP(F36,LOCALIZAÇÃO!A37:D113,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A37" s="49"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="52" t="str">
+        <f>IF(F37&lt;&gt;"",VLOOKUP(F37,LOCALIZAÇÃO!A38:D114,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A38" s="49"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="52" t="str">
+        <f>IF(F38&lt;&gt;"",VLOOKUP(F38,LOCALIZAÇÃO!A39:D115,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A39" s="49"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="52" t="str">
+        <f>IF(F39&lt;&gt;"",VLOOKUP(F39,LOCALIZAÇÃO!A40:D116,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A40" s="49"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="52" t="str">
+        <f>IF(F40&lt;&gt;"",VLOOKUP(F40,LOCALIZAÇÃO!A41:D117,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A41" s="49"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="52" t="str">
+        <f>IF(F41&lt;&gt;"",VLOOKUP(F41,LOCALIZAÇÃO!A42:D118,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A42" s="49"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="52" t="str">
+        <f>IF(F42&lt;&gt;"",VLOOKUP(F42,LOCALIZAÇÃO!A43:D119,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A43" s="49"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="52" t="str">
+        <f>IF(F43&lt;&gt;"",VLOOKUP(F43,LOCALIZAÇÃO!A44:D120,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A44" s="49"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="52" t="str">
+        <f>IF(F44&lt;&gt;"",VLOOKUP(F44,LOCALIZAÇÃO!A45:D121,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A45" s="49"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="52" t="str">
+        <f>IF(F45&lt;&gt;"",VLOOKUP(F45,LOCALIZAÇÃO!A46:D122,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A46" s="49"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="52" t="str">
+        <f>IF(F46&lt;&gt;"",VLOOKUP(F46,LOCALIZAÇÃO!A47:D123,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A47" s="49"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="52" t="str">
+        <f>IF(F47&lt;&gt;"",VLOOKUP(F47,LOCALIZAÇÃO!A48:D124,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A48" s="49"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="52" t="str">
+        <f>IF(F48&lt;&gt;"",VLOOKUP(F48,LOCALIZAÇÃO!A49:D125,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A49" s="49"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="51"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="52" t="str">
+        <f>IF(F49&lt;&gt;"",VLOOKUP(F49,LOCALIZAÇÃO!A50:D126,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A50" s="49"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="52" t="str">
+        <f>IF(F50&lt;&gt;"",VLOOKUP(F50,LOCALIZAÇÃO!A51:D127,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A51" s="49"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="52" t="str">
+        <f>IF(F51&lt;&gt;"",VLOOKUP(F51,LOCALIZAÇÃO!A52:D128,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A52" s="49"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="52" t="str">
+        <f>IF(F52&lt;&gt;"",VLOOKUP(F52,LOCALIZAÇÃO!A53:D129,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A53" s="49"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="51"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="52" t="str">
+        <f>IF(F53&lt;&gt;"",VLOOKUP(F53,LOCALIZAÇÃO!A54:D130,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A54" s="49"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="52" t="str">
+        <f>IF(F54&lt;&gt;"",VLOOKUP(F54,LOCALIZAÇÃO!A55:D131,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A55" s="49"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="52" t="str">
+        <f>IF(F55&lt;&gt;"",VLOOKUP(F55,LOCALIZAÇÃO!A56:D132,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A56" s="49"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="50"/>
+      <c r="G56" s="52" t="str">
+        <f>IF(F56&lt;&gt;"",VLOOKUP(F56,LOCALIZAÇÃO!A57:D133,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A57" s="49"/>
+      <c r="B57" s="50"/>
+      <c r="C57" s="51"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="50"/>
+      <c r="G57" s="52" t="str">
+        <f>IF(F57&lt;&gt;"",VLOOKUP(F57,LOCALIZAÇÃO!A58:D134,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A58" s="49"/>
+      <c r="B58" s="50"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="50"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="50"/>
+      <c r="G58" s="52" t="str">
+        <f>IF(F58&lt;&gt;"",VLOOKUP(F58,LOCALIZAÇÃO!A59:D135,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A59" s="49"/>
+      <c r="B59" s="50"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="52" t="str">
+        <f>IF(F59&lt;&gt;"",VLOOKUP(F59,LOCALIZAÇÃO!A60:D136,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A60" s="49"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="51"/>
+      <c r="D60" s="50"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="50"/>
+      <c r="G60" s="52" t="str">
+        <f>IF(F60&lt;&gt;"",VLOOKUP(F60,LOCALIZAÇÃO!A61:D137,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A61" s="49"/>
+      <c r="B61" s="50"/>
+      <c r="C61" s="51"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="52" t="str">
+        <f>IF(F61&lt;&gt;"",VLOOKUP(F61,LOCALIZAÇÃO!A62:D138,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A62" s="49"/>
+      <c r="B62" s="50"/>
+      <c r="C62" s="51"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="50"/>
+      <c r="F62" s="50"/>
+      <c r="G62" s="52" t="str">
+        <f>IF(F62&lt;&gt;"",VLOOKUP(F62,LOCALIZAÇÃO!A63:D139,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A63" s="49"/>
+      <c r="B63" s="50"/>
+      <c r="C63" s="51"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="52" t="str">
+        <f>IF(F63&lt;&gt;"",VLOOKUP(F63,LOCALIZAÇÃO!A64:D140,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A64" s="49"/>
+      <c r="B64" s="50"/>
+      <c r="C64" s="51"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="52" t="str">
+        <f>IF(F64&lt;&gt;"",VLOOKUP(F64,LOCALIZAÇÃO!A65:D141,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A65" s="49"/>
+      <c r="B65" s="50"/>
+      <c r="C65" s="51"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="50"/>
+      <c r="F65" s="50"/>
+      <c r="G65" s="52" t="str">
+        <f>IF(F65&lt;&gt;"",VLOOKUP(F65,LOCALIZAÇÃO!A66:D142,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A66" s="49"/>
+      <c r="B66" s="50"/>
+      <c r="C66" s="51"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="52" t="str">
+        <f>IF(F66&lt;&gt;"",VLOOKUP(F66,LOCALIZAÇÃO!A67:D143,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A67" s="49"/>
+      <c r="B67" s="50"/>
+      <c r="C67" s="51"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="52" t="str">
+        <f>IF(F67&lt;&gt;"",VLOOKUP(F67,LOCALIZAÇÃO!A68:D144,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A68" s="49"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="51"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="52" t="str">
+        <f>IF(F68&lt;&gt;"",VLOOKUP(F68,LOCALIZAÇÃO!A69:D145,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A69" s="49"/>
+      <c r="B69" s="50"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="52" t="str">
+        <f>IF(F69&lt;&gt;"",VLOOKUP(F69,LOCALIZAÇÃO!A70:D146,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A70" s="49"/>
+      <c r="B70" s="50"/>
+      <c r="C70" s="51"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="50"/>
+      <c r="F70" s="50"/>
+      <c r="G70" s="52" t="str">
+        <f>IF(F70&lt;&gt;"",VLOOKUP(F70,LOCALIZAÇÃO!A71:D147,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A71" s="49"/>
+      <c r="B71" s="50"/>
+      <c r="C71" s="51"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="50"/>
+      <c r="F71" s="50"/>
+      <c r="G71" s="52" t="str">
+        <f>IF(F71&lt;&gt;"",VLOOKUP(F71,LOCALIZAÇÃO!A72:D148,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A72" s="49"/>
+      <c r="B72" s="50"/>
+      <c r="C72" s="51"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="52" t="str">
+        <f>IF(F72&lt;&gt;"",VLOOKUP(F72,LOCALIZAÇÃO!A73:D149,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A73" s="49"/>
+      <c r="B73" s="50"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="52" t="str">
+        <f>IF(F73&lt;&gt;"",VLOOKUP(F73,LOCALIZAÇÃO!A74:D150,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A74" s="49"/>
+      <c r="B74" s="50"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="50"/>
+      <c r="F74" s="50"/>
+      <c r="G74" s="52" t="str">
+        <f>IF(F74&lt;&gt;"",VLOOKUP(F74,LOCALIZAÇÃO!A75:D151,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A75" s="49"/>
+      <c r="B75" s="50"/>
+      <c r="C75" s="51"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="52" t="str">
+        <f>IF(F75&lt;&gt;"",VLOOKUP(F75,LOCALIZAÇÃO!A76:D152,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A76" s="49"/>
+      <c r="B76" s="50"/>
+      <c r="C76" s="51"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="52" t="str">
+        <f>IF(F76&lt;&gt;"",VLOOKUP(F76,LOCALIZAÇÃO!A77:D153,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A77" s="49"/>
+      <c r="B77" s="50"/>
+      <c r="C77" s="51"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="50"/>
+      <c r="F77" s="50"/>
+      <c r="G77" s="52" t="str">
+        <f>IF(F77&lt;&gt;"",VLOOKUP(F77,LOCALIZAÇÃO!A78:D154,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A78" s="49"/>
+      <c r="B78" s="50"/>
+      <c r="C78" s="51"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="52" t="str">
+        <f>IF(F78&lt;&gt;"",VLOOKUP(F78,LOCALIZAÇÃO!A79:D155,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A79" s="49"/>
+      <c r="B79" s="50"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="52" t="str">
+        <f>IF(F79&lt;&gt;"",VLOOKUP(F79,LOCALIZAÇÃO!A80:D156,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A80" s="49"/>
+      <c r="B80" s="50"/>
+      <c r="C80" s="51"/>
+      <c r="D80" s="50"/>
+      <c r="E80" s="50"/>
+      <c r="F80" s="50"/>
+      <c r="G80" s="52" t="str">
+        <f>IF(F80&lt;&gt;"",VLOOKUP(F80,LOCALIZAÇÃO!A81:D157,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A81" s="49"/>
+      <c r="B81" s="50"/>
+      <c r="C81" s="51"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="50"/>
+      <c r="F81" s="50"/>
+      <c r="G81" s="52" t="str">
+        <f>IF(F81&lt;&gt;"",VLOOKUP(F81,LOCALIZAÇÃO!A82:D158,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A82" s="49"/>
+      <c r="B82" s="50"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="50"/>
+      <c r="E82" s="50"/>
+      <c r="F82" s="50"/>
+      <c r="G82" s="52" t="str">
+        <f>IF(F82&lt;&gt;"",VLOOKUP(F82,LOCALIZAÇÃO!A83:D159,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A83" s="49"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="50"/>
+      <c r="F83" s="50"/>
+      <c r="G83" s="52" t="str">
+        <f>IF(F83&lt;&gt;"",VLOOKUP(F83,LOCALIZAÇÃO!A84:D160,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A84" s="49"/>
+      <c r="B84" s="50"/>
+      <c r="C84" s="51"/>
+      <c r="D84" s="50"/>
+      <c r="E84" s="50"/>
+      <c r="F84" s="50"/>
+      <c r="G84" s="52" t="str">
+        <f>IF(F84&lt;&gt;"",VLOOKUP(F84,LOCALIZAÇÃO!A85:D161,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A85" s="49"/>
+      <c r="B85" s="50"/>
+      <c r="C85" s="51"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="50"/>
+      <c r="F85" s="50"/>
+      <c r="G85" s="52" t="str">
+        <f>IF(F85&lt;&gt;"",VLOOKUP(F85,LOCALIZAÇÃO!A86:D162,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A86" s="49"/>
+      <c r="B86" s="50"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="50"/>
+      <c r="E86" s="50"/>
+      <c r="F86" s="50"/>
+      <c r="G86" s="52" t="str">
+        <f>IF(F86&lt;&gt;"",VLOOKUP(F86,LOCALIZAÇÃO!A87:D163,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A87" s="49"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="50"/>
+      <c r="E87" s="50"/>
+      <c r="F87" s="50"/>
+      <c r="G87" s="52" t="str">
+        <f>IF(F87&lt;&gt;"",VLOOKUP(F87,LOCALIZAÇÃO!A88:D164,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A88" s="49"/>
+      <c r="B88" s="50"/>
+      <c r="C88" s="51"/>
+      <c r="D88" s="50"/>
+      <c r="E88" s="50"/>
+      <c r="F88" s="50"/>
+      <c r="G88" s="52" t="str">
+        <f>IF(F88&lt;&gt;"",VLOOKUP(F88,LOCALIZAÇÃO!A89:D165,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A89" s="49"/>
+      <c r="B89" s="50"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="50"/>
+      <c r="E89" s="50"/>
+      <c r="F89" s="50"/>
+      <c r="G89" s="52" t="str">
+        <f>IF(F89&lt;&gt;"",VLOOKUP(F89,LOCALIZAÇÃO!A90:D166,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A90" s="49"/>
+      <c r="B90" s="50"/>
+      <c r="C90" s="51"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="50"/>
+      <c r="F90" s="50"/>
+      <c r="G90" s="52" t="str">
+        <f>IF(F90&lt;&gt;"",VLOOKUP(F90,LOCALIZAÇÃO!A91:D167,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A91" s="49"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="51"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="52" t="str">
+        <f>IF(F91&lt;&gt;"",VLOOKUP(F91,LOCALIZAÇÃO!A92:D168,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A92" s="49"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="51"/>
+      <c r="D92" s="50"/>
+      <c r="E92" s="50"/>
+      <c r="F92" s="50"/>
+      <c r="G92" s="52" t="str">
+        <f>IF(F92&lt;&gt;"",VLOOKUP(F92,LOCALIZAÇÃO!A93:D169,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A93" s="49"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="51"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="50"/>
+      <c r="F93" s="50"/>
+      <c r="G93" s="52" t="str">
+        <f>IF(F93&lt;&gt;"",VLOOKUP(F93,LOCALIZAÇÃO!A94:D170,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A94" s="49"/>
+      <c r="B94" s="50"/>
+      <c r="C94" s="51"/>
+      <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="52" t="str">
+        <f>IF(F94&lt;&gt;"",VLOOKUP(F94,LOCALIZAÇÃO!A95:D171,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A95" s="49"/>
+      <c r="B95" s="50"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="50"/>
+      <c r="E95" s="50"/>
+      <c r="F95" s="50"/>
+      <c r="G95" s="52" t="str">
+        <f>IF(F95&lt;&gt;"",VLOOKUP(F95,LOCALIZAÇÃO!A96:D172,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A96" s="49"/>
+      <c r="B96" s="50"/>
+      <c r="C96" s="51"/>
+      <c r="D96" s="50"/>
+      <c r="E96" s="50"/>
+      <c r="F96" s="50"/>
+      <c r="G96" s="52" t="str">
+        <f>IF(F96&lt;&gt;"",VLOOKUP(F96,LOCALIZAÇÃO!A97:D173,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A97" s="49"/>
+      <c r="B97" s="50"/>
+      <c r="C97" s="51"/>
+      <c r="D97" s="50"/>
+      <c r="E97" s="50"/>
+      <c r="F97" s="50"/>
+      <c r="G97" s="52" t="str">
+        <f>IF(F97&lt;&gt;"",VLOOKUP(F97,LOCALIZAÇÃO!A98:D174,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A98" s="49"/>
+      <c r="B98" s="50"/>
+      <c r="C98" s="51"/>
+      <c r="D98" s="50"/>
+      <c r="E98" s="50"/>
+      <c r="F98" s="50"/>
+      <c r="G98" s="52" t="str">
+        <f>IF(F98&lt;&gt;"",VLOOKUP(F98,LOCALIZAÇÃO!A99:D175,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A99" s="49"/>
+      <c r="B99" s="50"/>
+      <c r="C99" s="51"/>
+      <c r="D99" s="50"/>
+      <c r="E99" s="50"/>
+      <c r="F99" s="50"/>
+      <c r="G99" s="52" t="str">
+        <f>IF(F99&lt;&gt;"",VLOOKUP(F99,LOCALIZAÇÃO!A100:D176,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="39.6" thickBot="1" x14ac:dyDescent="0.8">
+      <c r="A100" s="49"/>
+      <c r="B100" s="50"/>
+      <c r="C100" s="51"/>
+      <c r="D100" s="50"/>
+      <c r="E100" s="50"/>
+      <c r="F100" s="50"/>
+      <c r="G100" s="52" t="str">
+        <f>IF(F100&lt;&gt;"",VLOOKUP(F100,LOCALIZAÇÃO!A101:D177,4,FALSE),"")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
@@ -1513,19 +2810,19 @@
           <x14:formula1>
             <xm:f>ATRIBUIDO!$A$2:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>E2</xm:sqref>
+          <xm:sqref>E2:E100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C9A6595-EDA6-4FDD-BEE4-CFDBA6C2442B}">
           <x14:formula1>
-            <xm:f>TITULO!$A$2:$A$43</xm:f>
+            <xm:f>TITULO!$A$2:$A$45</xm:f>
           </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
+          <xm:sqref>A2:A100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{89F359FB-FF17-4F39-B13E-63860C6FF08E}">
           <x14:formula1>
             <xm:f>LOCALIZAÇÃO!$A$3:$A$79</xm:f>
           </x14:formula1>
-          <xm:sqref>F2</xm:sqref>
+          <xm:sqref>F2:F100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1534,6 +2831,263 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5070748A-A2E0-4296-9F3D-CFF9CF15F663}">
+  <dimension ref="A1:A45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="44.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="35" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="43" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A12" s="43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="43" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A17" s="43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="43" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="43" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A24" s="43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="43" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="43" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A29" s="43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="43" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A31" s="43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A32" s="43" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A33" s="43" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A34" s="43" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A36" s="43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="43" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="43" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="43" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A44" s="43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E63F0D1-1A9B-4BE8-A5E6-282F820024E3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37D8D50-0468-4BBA-939B-71687E16B50A}">
   <dimension ref="A1:A41"/>
   <sheetViews>
@@ -1541,158 +3095,158 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="1" max="1" width="45.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="35" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="42" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="43" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="43" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="43" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="43" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="43" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="43" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="43" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="43" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="43" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="43" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="43" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="43"/>
     </row>
-    <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="43"/>
     </row>
-    <row r="16" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="43"/>
     </row>
-    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="43"/>
     </row>
-    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="43"/>
     </row>
-    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="43"/>
     </row>
-    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="43"/>
     </row>
-    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="43"/>
     </row>
-    <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="43"/>
     </row>
-    <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="43"/>
     </row>
-    <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="43"/>
     </row>
-    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="43"/>
     </row>
-    <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="43"/>
     </row>
-    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="43"/>
     </row>
-    <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="43"/>
     </row>
-    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="43"/>
     </row>
-    <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="43"/>
     </row>
-    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="43"/>
     </row>
-    <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="43"/>
     </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="43"/>
     </row>
-    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="43"/>
     </row>
-    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="43"/>
     </row>
-    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="43"/>
     </row>
-    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="43"/>
     </row>
-    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="43"/>
     </row>
-    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="43"/>
     </row>
-    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="43"/>
     </row>
-    <row r="41" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="44"/>
     </row>
   </sheetData>
@@ -1700,255 +3254,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5070748A-A2E0-4296-9F3D-CFF9CF15F663}">
-  <dimension ref="A1:A43"/>
-  <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="43" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="43" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="43" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="43" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="43" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="43" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="43" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="43" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="43" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="43" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="43" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="43" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="43" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="43" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="43" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="43" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="43" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="43" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="43" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="43" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="43" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="43" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="43" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="43" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="43" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="43" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="43" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="43" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="43" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="43" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="44" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377FF143-C3F8-4C93-9956-8A72982D22B7}">
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="4" max="4" width="133.85546875" customWidth="1"/>
+    <col min="1" max="1" width="48.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.88671875" customWidth="1"/>
+    <col min="4" max="4" width="133.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1959,11 +3280,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
@@ -1974,7 +3295,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
@@ -1985,7 +3306,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -1996,7 +3317,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
@@ -2007,7 +3328,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
@@ -2018,7 +3339,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -2029,7 +3350,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>18</v>
       </c>
@@ -2040,7 +3361,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
@@ -2051,7 +3372,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
@@ -2062,7 +3383,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
@@ -2073,7 +3394,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>23</v>
       </c>
@@ -2084,7 +3405,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>24</v>
       </c>
@@ -2095,7 +3416,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
@@ -2106,7 +3427,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>26</v>
       </c>
@@ -2117,7 +3438,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>27</v>
       </c>
@@ -2128,7 +3449,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>28</v>
       </c>
@@ -2139,7 +3460,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>29</v>
       </c>
@@ -2150,7 +3471,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
         <v>30</v>
       </c>
@@ -2161,7 +3482,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>32</v>
       </c>
@@ -2172,7 +3493,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>33</v>
       </c>
@@ -2183,7 +3504,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>34</v>
       </c>
@@ -2194,7 +3515,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>35</v>
       </c>
@@ -2205,7 +3526,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>36</v>
       </c>
@@ -2216,7 +3537,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>37</v>
       </c>
@@ -2227,7 +3548,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>39</v>
       </c>
@@ -2238,7 +3559,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>40</v>
       </c>
@@ -2249,7 +3570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>41</v>
       </c>
@@ -2260,7 +3581,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>42</v>
       </c>
@@ -2271,7 +3592,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>43</v>
       </c>
@@ -2282,7 +3603,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>44</v>
       </c>
@@ -2293,7 +3614,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A33" s="33" t="s">
         <v>96</v>
       </c>
@@ -2304,7 +3625,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>45</v>
       </c>
@@ -2315,7 +3636,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>46</v>
       </c>
@@ -2326,7 +3647,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>48</v>
       </c>
@@ -2337,7 +3658,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>49</v>
       </c>
@@ -2348,7 +3669,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>50</v>
       </c>
@@ -2359,7 +3680,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>51</v>
       </c>
@@ -2370,7 +3691,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>52</v>
       </c>
@@ -2381,7 +3702,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A41" s="23" t="s">
         <v>53</v>
       </c>
@@ -2392,7 +3713,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="11" t="s">
         <v>54</v>
       </c>
@@ -2403,7 +3724,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>55</v>
       </c>
@@ -2414,7 +3735,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>57</v>
       </c>
@@ -2425,7 +3746,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>58</v>
       </c>
@@ -2436,7 +3757,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>59</v>
       </c>
@@ -2447,7 +3768,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>60</v>
       </c>
@@ -2458,7 +3779,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>61</v>
       </c>
@@ -2469,7 +3790,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>62</v>
       </c>
@@ -2480,7 +3801,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>63</v>
       </c>
@@ -2491,7 +3812,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>64</v>
       </c>
@@ -2502,7 +3823,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>65</v>
       </c>
@@ -2513,7 +3834,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
         <v>66</v>
       </c>
@@ -2524,7 +3845,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
         <v>67</v>
       </c>
@@ -2535,7 +3856,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A55" s="13" t="s">
         <v>68</v>
       </c>
@@ -2546,7 +3867,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
         <v>70</v>
       </c>
@@ -2557,7 +3878,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>71</v>
       </c>
@@ -2568,7 +3889,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>72</v>
       </c>
@@ -2579,7 +3900,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>73</v>
       </c>
@@ -2590,7 +3911,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>74</v>
       </c>
@@ -2601,7 +3922,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>75</v>
       </c>
@@ -2612,7 +3933,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>76</v>
       </c>
@@ -2623,7 +3944,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A63" s="26" t="s">
         <v>77</v>
       </c>
@@ -2634,7 +3955,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
         <v>79</v>
       </c>
@@ -2645,7 +3966,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A65" s="28" t="s">
         <v>80</v>
       </c>
@@ -2656,7 +3977,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A66" s="29" t="s">
         <v>82</v>
       </c>
@@ -2667,7 +3988,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A67" s="29" t="s">
         <v>83</v>
       </c>
@@ -2678,7 +3999,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A68" s="29" t="s">
         <v>84</v>
       </c>
@@ -2689,7 +4010,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A69" s="29" t="s">
         <v>85</v>
       </c>
@@ -2700,7 +4021,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A70" s="29" t="s">
         <v>86</v>
       </c>
@@ -2711,7 +4032,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="30" t="s">
         <v>87</v>
       </c>
@@ -2722,7 +4043,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>88</v>
       </c>
@@ -2733,7 +4054,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A73" s="15" t="s">
         <v>90</v>
       </c>
@@ -2744,7 +4065,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A74" s="15" t="s">
         <v>91</v>
       </c>
@@ -2755,7 +4076,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="31" t="s">
         <v>92</v>
       </c>
@@ -2766,7 +4087,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A76" s="15" t="s">
         <v>93</v>
       </c>
@@ -2777,7 +4098,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="21" x14ac:dyDescent="0.3">
       <c r="A77" s="15" t="s">
         <v>94</v>
       </c>
@@ -2788,7 +4109,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="11" t="s">
         <v>95</v>
       </c>
@@ -2799,7 +4120,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="36" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Atualização do scrpit - Adicionando interface
- Escolha de planilha
- Escolhe de navegador
- Interface
</commit_message>
<xml_diff>
--- a/chamados.xlsx
+++ b/chamados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DSTIC\Documents\AbrirChamadosSua\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\kali-linux\home\felipesouza\Documents\projetoChmadosSua\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA5764-A9A1-445D-B6D4-6D533FE75943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B0A4FC-2E84-465B-A235-4F5F6C710698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="1035" windowWidth="15330" windowHeight="10800" xr2:uid="{00F37107-7D40-4ADB-921F-DDFA62B1AA1C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00F37107-7D40-4ADB-921F-DDFA62B1AA1C}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="LOCALIZAÇÃO" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MAIN!$A$1:$G$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MAIN!$A$1:$G$99</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -76,30 +76,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{B89011F1-16F2-479B-830C-046990E0E26A}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t>Felipe Souza:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Segoe UI"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -113,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="295">
   <si>
     <t>TITULO</t>
   </si>
@@ -184,120 +160,9 @@
     <t>Solerne</t>
   </si>
   <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Rosangela Pimentel</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOMES PARA SCRIPT </t>
   </si>
   <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Policlínica Barral y Barral &gt; Unidade de Saúde da Família Rosa Maria dos Santos</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; USF Raimunda Dionizio da Silva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; Unidade de Saúde da Família Maria de Fátima </t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; UBS Jose Gomes de Oliveira</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; UBS Francisco Constancio da Silva</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; UBS Aeroporto velho</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade de Saúde da Família Triângulo Novo</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade de Saúde da Família Recanto</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; USF Maria de Jesus Andrade</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; Unidade de Saúde da Família Maria de Fátima</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade Básica de Saúde Francisca Barbosa Guerra</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Unidades de Saúde &gt; Divisão de Apoio Diagnostico &gt; Centro de Apoio e Diagnóstico I</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; UBS Maria Barroso da Silva</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; Unidade Básica de Saúde Dr. Raimundo Moreira</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Augusto Hidalgo &gt; Unidade Básica de Saúde Maria Verônica Rodrigues de Souza</t>
-  </si>
-  <si>
-    <t>Diretoria do Fundo Municipal de Saúde &gt; Departamento de Recursos Logísticos &gt; Divisão de Transporte</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Policlínica Barral y Barral &gt; Unidade de Saúde da Família Nímio Isfram Martinez</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Formação do Tucumã &gt; Unidade de Saúde da Família Mocinha Magalhães</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Rosangela Pimentel &gt; UBS Máximo Diogo Magalhães</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Rosangela Pimentel &gt; UBS Mariano Gonzaga</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Formação do Tucumã &gt; Unidade de Saúde da Família Rui Lino</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Vila Ivonete</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Roney Meireles</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Roney Meireles &gt; UBS Platilde Oliveira da Silva</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Vila Ivonete &gt; Unidade Básica de Saúde Luana Souza de Freitas</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Roney Meireles &gt; Unidade de Saúde da Família Elpidio Moreira Souza</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Redes de Atenção &gt; Divisão de Apoio Diagnóstico &gt; Núcleo do Centro de Apoio e Diagnóstico de Imagem</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Unidade Básica de Saúde &gt; sáude/unidade básica Equipe Multiprofissional de Atenção Domiciliar (EMAD)</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP Eduardo Assmar</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Ary Rodrigues</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Mário Maia</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; UBS Maria Sebastiana Bernardo</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Ary Rodrigues &gt; UBS Maria Aurea Vilela dos Santos</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade de Saúde da Família Benfica</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Ary Rodrigues &gt; USF Antenor Francisco Ramos</t>
-  </si>
-  <si>
     <t>VISITA TÉCNICA</t>
   </si>
   <si>
@@ -421,81 +286,9 @@
     <t>TÍTULOS DOS CHAMADOS</t>
   </si>
   <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade de Saúde da Família Ana Rosa de Amorin</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade de Saúde da Família Agripina Lindoso</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Redes de Atenção &gt; Divisão de Rede de Atenção Psicossocial &gt; Núcleo de Unidade de Acolhimento ao Adulto</t>
-  </si>
-  <si>
-    <t>Diretoria de Vigilância em Saúde &gt; Departamento de Controle de Zoonoses</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade Básica de Saúde Valdeisa Correia Valdez</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; UBS Tereza Paz Rosas</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Souza Araújo &gt; Unidade de Saúde da Família Maria Sofia</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade Básica de Saúde Manoel Alves Bezerra Neto</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Souza Araújo &gt; Unidade de Saúde da Família Belo Jardim III</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Unidade de Saúde da Família Belo Jardim I</t>
-  </si>
-  <si>
     <t>Diretoria de Vigilância em Saúde</t>
   </si>
   <si>
-    <t>Diretoria de Vigilância em Saúde &gt; Departamento de Vigilância Epidemiológica e Ambiental</t>
-  </si>
-  <si>
-    <t>iretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP São Francisco</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP São Francisco &gt; UBS Vitória</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Deusimar Pinheiro da Silva &gt; USF Luiz Gonzaga de Lima Carneiro</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; URAP São Francisco &gt; Unidade de Saúde da Família Adalberto Aragão</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Deusimar Pinheiro da Silva</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Policlínica Barral y Barral &gt; UBS Gentil Perdomo da Rocha</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Policlínica Barral y Barral</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Diretoria de Gestão &gt; Departamento de Administração &gt; Divisão de Material e Patrimônio</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Redes de Atenção &gt; Divisão de Rede de Atenção Psicossocial &gt; Núcleo Mundo Azul</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Assistência Farmacêutica &gt; Divisão de Medicamentos</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Assistência Farmacêutica</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de URAP e Centro de Saúde &gt; Centro de Saúde Drª Claudia Vitorino &gt; Centro de Especialidade Odontológica - CEO</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Unidade Básica de Saúde &gt; Unidades de Saúde da Família</t>
-  </si>
-  <si>
     <t>NOME DOS TÉCNICOS</t>
   </si>
   <si>
@@ -862,54 +655,15 @@
     <t>Diretoria de Assistência a Saúde</t>
   </si>
   <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Redes de Atenção</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Saúde Bucal</t>
-  </si>
-  <si>
-    <t>Diretoria de Assistência a Saúde &gt; Departamento de Unidade Básica de Saúde &gt; Centro de Atenção ao Autista</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Fundo Vinculado &gt; Fundo Municipal de Saúde</t>
-  </si>
-  <si>
     <t>Diretoria de Regulação, Controle e Avaliação</t>
   </si>
   <si>
-    <t>Diretoria de Regulação, Controle e Avaliação &gt; Departamento de Processos de Regulação, Controle e Avaliação</t>
-  </si>
-  <si>
     <t>Diretoria do Fundo Municipal de Saúde</t>
   </si>
   <si>
-    <t>Diretoria do Fundo Municipal de Saúde &gt; Departamento de Recursos Logísticos &gt; Divisão de Suporte e Tecnologia da Informação</t>
-  </si>
-  <si>
     <t>Secretario - SEMSA</t>
   </si>
   <si>
-    <t>Secretario - SEMSA &gt; Assessoria Jurídica</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Assessoria Técnica</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Chefia de Gabinete</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Chefia de Gabinete &gt; Assessoria de Planejamento, Convênios e Projetos</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Chefia de Gabinete &gt; Unidade de Controle Interno e Auditoria</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Chefia de Gabinete &gt; Unidade de Ouvidoria</t>
-  </si>
-  <si>
-    <t>Secretario - SEMSA &gt; Diretoria de Gestão</t>
-  </si>
-  <si>
     <t>SEMA - CONSELHO MUNICIPAL DE SAÚDE</t>
   </si>
   <si>
@@ -973,13 +727,253 @@
     <t>CONTAGEM DE COMPUTADORES</t>
   </si>
   <si>
-    <t xml:space="preserve">Problema: Fazer contagem de computadores Unidade: SEMSA - Administrativo </t>
-  </si>
-  <si>
     <t xml:space="preserve"> USF RAIMUNDA DIONIZIO DA SILVA</t>
   </si>
   <si>
     <t>SEMSA - DETI</t>
+  </si>
+  <si>
+    <t>SEMSA - DELC</t>
+  </si>
+  <si>
+    <t>SUPORTE GMUS</t>
+  </si>
+  <si>
+    <t>COMPARTILHAMENTO DE PASTA</t>
+  </si>
+  <si>
+    <t>Divisão de Suporte e Tecnologia da Informação</t>
+  </si>
+  <si>
+    <t>Centro de Atenção ao Autista</t>
+  </si>
+  <si>
+    <t>Divisão de Contratos e Licitações</t>
+  </si>
+  <si>
+    <t>Departamento de Processos de Regulação, Controle e Avaliação</t>
+  </si>
+  <si>
+    <t>Fundo Municipal de Saúde</t>
+  </si>
+  <si>
+    <t>Departamento de Redes de Atenção</t>
+  </si>
+  <si>
+    <t>Departamento de Saúde Bucal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assessoria Jurídica</t>
+  </si>
+  <si>
+    <t>Assessoria Técnica</t>
+  </si>
+  <si>
+    <t>Chefia de Gabinete</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Assessoria de Planejamento, Convênios e Projetos</t>
+  </si>
+  <si>
+    <t>Unidade de Controle Interno e Auditoria</t>
+  </si>
+  <si>
+    <t>Unidade de Ouvidoria</t>
+  </si>
+  <si>
+    <t>Diretoria de Gestão</t>
+  </si>
+  <si>
+    <t>USF Raimunda Dionizio da Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidade de Saúde da Família Maria de Fátima </t>
+  </si>
+  <si>
+    <t>UBS Jose Gomes de Oliveira</t>
+  </si>
+  <si>
+    <t>UBS Francisco Constancio da Silva</t>
+  </si>
+  <si>
+    <t>UBS Aeroporto velho</t>
+  </si>
+  <si>
+    <t>Unidades de Saúde da Família</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Triângulo Novo</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Recanto</t>
+  </si>
+  <si>
+    <t>USF Maria de Jesus Andrade</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Maria de Fátima</t>
+  </si>
+  <si>
+    <t>Centro de Especialidade Odontológica - CEO</t>
+  </si>
+  <si>
+    <t>Departamento de Assistência Farmacêutica</t>
+  </si>
+  <si>
+    <t>Departamento de Assistência Farmacêutica &gt; Divisão de Medicamentos</t>
+  </si>
+  <si>
+    <t>Núcleo Mundo Azul</t>
+  </si>
+  <si>
+    <t>Divisão de Material e Patrimônio</t>
+  </si>
+  <si>
+    <t>Departamento de URAP e Centro de Saúde</t>
+  </si>
+  <si>
+    <t>Unidade Básica de Saúde Francisca Barbosa Guerra</t>
+  </si>
+  <si>
+    <t>Policlínica Barral y Barral</t>
+  </si>
+  <si>
+    <t>Policlínica Barral y Barral &gt; UBS Gentil Perdomo da Rocha</t>
+  </si>
+  <si>
+    <t>Centro de Saúde Deusimar Pinheiro da Silva</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Adalberto Aragão</t>
+  </si>
+  <si>
+    <t>USF Luiz Gonzaga de Lima Carneiro</t>
+  </si>
+  <si>
+    <t>UBS Vitória</t>
+  </si>
+  <si>
+    <t>URAP São Francisco</t>
+  </si>
+  <si>
+    <t>Departamento de Vigilância Epidemiológica e Ambiental</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Belo Jardim I</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Belo Jardim III</t>
+  </si>
+  <si>
+    <t>Unidade Básica de Saúde Manoel Alves Bezerra Neto</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Maria Sofia</t>
+  </si>
+  <si>
+    <t>UBS Tereza Paz Rosas</t>
+  </si>
+  <si>
+    <t>Unidade Básica de Saúde Valdeisa Correia Valdez</t>
+  </si>
+  <si>
+    <t>Departamento de Controle de Zoonoses</t>
+  </si>
+  <si>
+    <t>Núcleo de Unidade de Acolhimento ao Adulto</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Agripina Lindoso</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Ana Rosa de Amorin</t>
+  </si>
+  <si>
+    <t>USF Antenor Francisco Ramos</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Benfica</t>
+  </si>
+  <si>
+    <t>UBS Maria Aurea Vilela dos Santos</t>
+  </si>
+  <si>
+    <t>UBS Maria Sebastiana Bernardo</t>
+  </si>
+  <si>
+    <t>Centro de Saúde Mário Maia</t>
+  </si>
+  <si>
+    <t>Centro de Saúde Ary Rodrigues</t>
+  </si>
+  <si>
+    <t>URAP Eduardo Assmar</t>
+  </si>
+  <si>
+    <t>sáude/unidade básica Equipe Multiprofissional de Atenção Domiciliar (EMAD)</t>
+  </si>
+  <si>
+    <t>Divisão de Apoio Diagnostico &gt; Centro de Apoio e Diagnóstico I</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Elpidio Moreira Souza</t>
+  </si>
+  <si>
+    <t>Unidade Básica de Saúde Luana Souza de Freitas</t>
+  </si>
+  <si>
+    <t>UBS Platilde Oliveira da Silva</t>
+  </si>
+  <si>
+    <t>URAP Roney Meireles</t>
+  </si>
+  <si>
+    <t>Centro de Saúde Vila Ivonete</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Rui Lino</t>
+  </si>
+  <si>
+    <t>UBS Mariano Gonzaga</t>
+  </si>
+  <si>
+    <t>UBS Máximo Diogo Magalhães</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Mocinha Magalhães</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Nímio Isfram Martinez</t>
+  </si>
+  <si>
+    <t>Unidade de Saúde da Família Rosa Maria dos Santos</t>
+  </si>
+  <si>
+    <t>Centro de Saúde Rosangela Pimentel</t>
+  </si>
+  <si>
+    <t>Unidade Básica de Saúde Maria Verônica Rodrigues de Souza</t>
+  </si>
+  <si>
+    <t>Unidade Básica de Saúde Dr. Raimundo Moreira</t>
+  </si>
+  <si>
+    <t>Departamento de Recursos Logísticos &gt; Divisão de Transporte</t>
+  </si>
+  <si>
+    <t>UBS Maria Barroso da Silva</t>
+  </si>
+  <si>
+    <t>Núcleo do Centro de Apoio e Diagnóstico de Imagem</t>
+  </si>
+  <si>
+    <t>SEMSA - DIRETORIA DE CUIDADOS À SAÚDE DA COMUNIDADE</t>
+  </si>
+  <si>
+    <t>CONFECÇÃO CABO DE REDE</t>
+  </si>
+  <si>
+    <t>Problema: Confecção de cabo de rede Local: SEMSA - Administrativo - Planejamento</t>
   </si>
 </sst>
 </file>
@@ -989,7 +983,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,19 +1013,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="26"/>
       <color indexed="81"/>
@@ -1056,14 +1037,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1452,70 +1425,69 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1525,6 +1497,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1659,8 +1634,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{12AAC97F-3921-4801-A0DD-A63DA3723794}" name="localização" displayName="localização" ref="A1:C100" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="A1:C100" xr:uid="{12AAC97F-3921-4801-A0DD-A63DA3723794}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{12AAC97F-3921-4801-A0DD-A63DA3723794}" name="localização" displayName="localização" ref="A1:C102" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:C102" xr:uid="{12AAC97F-3921-4801-A0DD-A63DA3723794}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{13DBE4DB-F779-4F7C-990A-74B0D65BCA7D}" name="UNIDADES DE SAÚDE" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{66A6F666-3602-4B17-8ED2-509311D1FFF5}" name="Técnico" dataDxfId="1"/>
@@ -1987,21 +1962,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D6CDD5-46C2-41B8-B947-C28F11FD0B44}">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="39" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
@@ -2012,7 +1987,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>2</v>
@@ -2021,7 +1996,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>139</v>
+        <v>78</v>
       </c>
       <c r="G1" s="13" t="s">
         <v>6</v>
@@ -2029,26 +2004,27 @@
     </row>
     <row r="2" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C2" s="7">
-        <v>45834.541666666664</v>
+        <v>45840.520833333336</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>5</v>
+      <c r="E2" s="45" t="str">
+        <f t="shared" ref="E2:E65" si="0">IF(A2&lt;&gt;"","FELIPE PINTO DE SOUZA","")</f>
+        <v>FELIPE PINTO DE SOUZA</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>288</v>
+        <v>207</v>
       </c>
       <c r="G2" s="8" t="str">
         <f>IF(F2&lt;&gt;"",VLOOKUP(F2,localização[],3,FALSE),"")</f>
-        <v>Diretoria do Fundo Municipal de Saúde &gt; Departamento de Recursos Logísticos &gt; Divisão de Suporte e Tecnologia da Informação</v>
+        <v xml:space="preserve"> Assessoria de Planejamento, Convênios e Projetos</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2056,7 +2032,10 @@
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="E3" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F3" s="6"/>
       <c r="G3" s="8" t="str">
         <f>IF(F3&lt;&gt;"",VLOOKUP(F3,localização[],3,FALSE),"")</f>
@@ -2068,7 +2047,10 @@
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="8" t="str">
         <f>IF(F4&lt;&gt;"",VLOOKUP(F4,localização[],3,FALSE),"")</f>
@@ -2080,7 +2062,10 @@
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F5" s="6"/>
       <c r="G5" s="8" t="str">
         <f>IF(F5&lt;&gt;"",VLOOKUP(F5,localização[],3,FALSE),"")</f>
@@ -2092,7 +2077,10 @@
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="8" t="str">
         <f>IF(F6&lt;&gt;"",VLOOKUP(F6,localização[],3,FALSE),"")</f>
@@ -2104,7 +2092,10 @@
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="8" t="str">
         <f>IF(F7&lt;&gt;"",VLOOKUP(F7,localização[],3,FALSE),"")</f>
@@ -2116,32 +2107,41 @@
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="8" t="str">
         <f>IF(F8&lt;&gt;"",VLOOKUP(F8,localização[],3,FALSE),"")</f>
         <v/>
       </c>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
-      <c r="C9" s="16"/>
+      <c r="C9" s="7"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="8" t="str">
         <f>IF(F9&lt;&gt;"",VLOOKUP(F9,localização[],3,FALSE),"")</f>
         <v/>
       </c>
-      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="7"/>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="8" t="str">
         <f>IF(F10&lt;&gt;"",VLOOKUP(F10,localização[],3,FALSE),"")</f>
@@ -2153,19 +2153,19 @@
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="8" t="str">
-        <f>IF(F11&lt;&gt;"",VLOOKUP(F11,localização[],3,FALSE),"")</f>
-        <v/>
-      </c>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="E12" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8" t="str">
         <f>IF(F12&lt;&gt;"",VLOOKUP(F12,localização[],3,FALSE),"")</f>
@@ -2177,7 +2177,10 @@
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="E13" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8" t="str">
         <f>IF(F13&lt;&gt;"",VLOOKUP(F13,localização[],3,FALSE),"")</f>
@@ -2189,7 +2192,10 @@
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="E14" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8" t="str">
         <f>IF(F14&lt;&gt;"",VLOOKUP(F14,localização[],3,FALSE),"")</f>
@@ -2201,7 +2207,10 @@
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="E15" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="8" t="str">
         <f>IF(F15&lt;&gt;"",VLOOKUP(F15,localização[],3,FALSE),"")</f>
@@ -2213,7 +2222,10 @@
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="E16" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="8" t="str">
         <f>IF(F16&lt;&gt;"",VLOOKUP(F16,localização[],3,FALSE),"")</f>
@@ -2225,7 +2237,10 @@
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="8" t="str">
         <f>IF(F17&lt;&gt;"",VLOOKUP(F17,localização[],3,FALSE),"")</f>
@@ -2237,7 +2252,10 @@
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="8" t="str">
         <f>IF(F18&lt;&gt;"",VLOOKUP(F18,localização[],3,FALSE),"")</f>
@@ -2249,7 +2267,10 @@
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="8" t="str">
         <f>IF(F19&lt;&gt;"",VLOOKUP(F19,localização[],3,FALSE),"")</f>
@@ -2261,7 +2282,10 @@
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="8" t="str">
         <f>IF(F20&lt;&gt;"",VLOOKUP(F20,localização[],3,FALSE),"")</f>
@@ -2273,7 +2297,10 @@
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="8" t="str">
         <f>IF(F21&lt;&gt;"",VLOOKUP(F21,localização[],3,FALSE),"")</f>
@@ -2285,7 +2312,10 @@
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22" s="8" t="str">
         <f>IF(F22&lt;&gt;"",VLOOKUP(F22,localização[],3,FALSE),"")</f>
@@ -2297,7 +2327,10 @@
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="8" t="str">
         <f>IF(F23&lt;&gt;"",VLOOKUP(F23,localização[],3,FALSE),"")</f>
@@ -2309,7 +2342,10 @@
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="8" t="str">
         <f>IF(F24&lt;&gt;"",VLOOKUP(F24,localização[],3,FALSE),"")</f>
@@ -2321,7 +2357,10 @@
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="8" t="str">
         <f>IF(F25&lt;&gt;"",VLOOKUP(F25,localização[],3,FALSE),"")</f>
@@ -2333,7 +2372,10 @@
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="E26" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="8" t="str">
         <f>IF(F26&lt;&gt;"",VLOOKUP(F26,localização[],3,FALSE),"")</f>
@@ -2345,7 +2387,10 @@
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="E27" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="8" t="str">
         <f>IF(F27&lt;&gt;"",VLOOKUP(F27,localização[],3,FALSE),"")</f>
@@ -2357,7 +2402,10 @@
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="E28" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="8" t="str">
         <f>IF(F28&lt;&gt;"",VLOOKUP(F28,localização[],3,FALSE),"")</f>
@@ -2369,7 +2417,10 @@
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="E29" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="8" t="str">
         <f>IF(F29&lt;&gt;"",VLOOKUP(F29,localização[],3,FALSE),"")</f>
@@ -2381,7 +2432,10 @@
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="E30" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F30" s="6"/>
       <c r="G30" s="8" t="str">
         <f>IF(F30&lt;&gt;"",VLOOKUP(F30,localização[],3,FALSE),"")</f>
@@ -2393,7 +2447,10 @@
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F31" s="6"/>
       <c r="G31" s="8" t="str">
         <f>IF(F31&lt;&gt;"",VLOOKUP(F31,localização[],3,FALSE),"")</f>
@@ -2405,7 +2462,10 @@
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="E32" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F32" s="6"/>
       <c r="G32" s="8" t="str">
         <f>IF(F32&lt;&gt;"",VLOOKUP(F32,localização[],3,FALSE),"")</f>
@@ -2417,7 +2477,10 @@
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
       <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="E33" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F33" s="6"/>
       <c r="G33" s="8" t="str">
         <f>IF(F33&lt;&gt;"",VLOOKUP(F33,localização[],3,FALSE),"")</f>
@@ -2429,7 +2492,10 @@
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
       <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="E34" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F34" s="6"/>
       <c r="G34" s="8" t="str">
         <f>IF(F34&lt;&gt;"",VLOOKUP(F34,localização[],3,FALSE),"")</f>
@@ -2441,7 +2507,10 @@
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="8" t="str">
         <f>IF(F35&lt;&gt;"",VLOOKUP(F35,localização[],3,FALSE),"")</f>
@@ -2453,7 +2522,10 @@
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
       <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="E36" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F36" s="6"/>
       <c r="G36" s="8" t="str">
         <f>IF(F36&lt;&gt;"",VLOOKUP(F36,localização[],3,FALSE),"")</f>
@@ -2465,7 +2537,10 @@
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
       <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="E37" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F37" s="6"/>
       <c r="G37" s="8" t="str">
         <f>IF(F37&lt;&gt;"",VLOOKUP(F37,localização[],3,FALSE),"")</f>
@@ -2477,7 +2552,10 @@
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
       <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="E38" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="8" t="str">
         <f>IF(F38&lt;&gt;"",VLOOKUP(F38,localização[],3,FALSE),"")</f>
@@ -2489,7 +2567,10 @@
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
       <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="E39" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F39" s="6"/>
       <c r="G39" s="8" t="str">
         <f>IF(F39&lt;&gt;"",VLOOKUP(F39,localização[],3,FALSE),"")</f>
@@ -2501,7 +2582,10 @@
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
       <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="E40" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="8" t="str">
         <f>IF(F40&lt;&gt;"",VLOOKUP(F40,localização[],3,FALSE),"")</f>
@@ -2513,7 +2597,10 @@
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
       <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="E41" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F41" s="6"/>
       <c r="G41" s="8" t="str">
         <f>IF(F41&lt;&gt;"",VLOOKUP(F41,localização[],3,FALSE),"")</f>
@@ -2525,7 +2612,10 @@
       <c r="B42" s="6"/>
       <c r="C42" s="7"/>
       <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="E42" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F42" s="6"/>
       <c r="G42" s="8" t="str">
         <f>IF(F42&lt;&gt;"",VLOOKUP(F42,localização[],3,FALSE),"")</f>
@@ -2537,7 +2627,10 @@
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
       <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="E43" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F43" s="6"/>
       <c r="G43" s="8" t="str">
         <f>IF(F43&lt;&gt;"",VLOOKUP(F43,localização[],3,FALSE),"")</f>
@@ -2549,7 +2642,10 @@
       <c r="B44" s="6"/>
       <c r="C44" s="7"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F44" s="6"/>
       <c r="G44" s="8" t="str">
         <f>IF(F44&lt;&gt;"",VLOOKUP(F44,localização[],3,FALSE),"")</f>
@@ -2561,7 +2657,10 @@
       <c r="B45" s="6"/>
       <c r="C45" s="7"/>
       <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="E45" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="8" t="str">
         <f>IF(F45&lt;&gt;"",VLOOKUP(F45,localização[],3,FALSE),"")</f>
@@ -2573,7 +2672,10 @@
       <c r="B46" s="6"/>
       <c r="C46" s="7"/>
       <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F46" s="6"/>
       <c r="G46" s="8" t="str">
         <f>IF(F46&lt;&gt;"",VLOOKUP(F46,localização[],3,FALSE),"")</f>
@@ -2585,7 +2687,10 @@
       <c r="B47" s="6"/>
       <c r="C47" s="7"/>
       <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="8" t="str">
         <f>IF(F47&lt;&gt;"",VLOOKUP(F47,localização[],3,FALSE),"")</f>
@@ -2597,7 +2702,10 @@
       <c r="B48" s="6"/>
       <c r="C48" s="7"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="E48" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="8" t="str">
         <f>IF(F48&lt;&gt;"",VLOOKUP(F48,localização[],3,FALSE),"")</f>
@@ -2609,7 +2717,10 @@
       <c r="B49" s="6"/>
       <c r="C49" s="7"/>
       <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+      <c r="E49" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="8" t="str">
         <f>IF(F49&lt;&gt;"",VLOOKUP(F49,localização[],3,FALSE),"")</f>
@@ -2621,7 +2732,10 @@
       <c r="B50" s="6"/>
       <c r="C50" s="7"/>
       <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="E50" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="8" t="str">
         <f>IF(F50&lt;&gt;"",VLOOKUP(F50,localização[],3,FALSE),"")</f>
@@ -2633,7 +2747,10 @@
       <c r="B51" s="6"/>
       <c r="C51" s="7"/>
       <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="E51" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="8" t="str">
         <f>IF(F51&lt;&gt;"",VLOOKUP(F51,localização[],3,FALSE),"")</f>
@@ -2645,7 +2762,10 @@
       <c r="B52" s="6"/>
       <c r="C52" s="7"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="E52" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="8" t="str">
         <f>IF(F52&lt;&gt;"",VLOOKUP(F52,localização[],3,FALSE),"")</f>
@@ -2657,7 +2777,10 @@
       <c r="B53" s="6"/>
       <c r="C53" s="7"/>
       <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+      <c r="E53" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="8" t="str">
         <f>IF(F53&lt;&gt;"",VLOOKUP(F53,localização[],3,FALSE),"")</f>
@@ -2669,7 +2792,10 @@
       <c r="B54" s="6"/>
       <c r="C54" s="7"/>
       <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="E54" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F54" s="6"/>
       <c r="G54" s="8" t="str">
         <f>IF(F54&lt;&gt;"",VLOOKUP(F54,localização[],3,FALSE),"")</f>
@@ -2681,7 +2807,10 @@
       <c r="B55" s="6"/>
       <c r="C55" s="7"/>
       <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+      <c r="E55" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F55" s="6"/>
       <c r="G55" s="8" t="str">
         <f>IF(F55&lt;&gt;"",VLOOKUP(F55,localização[],3,FALSE),"")</f>
@@ -2693,7 +2822,10 @@
       <c r="B56" s="6"/>
       <c r="C56" s="7"/>
       <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="E56" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F56" s="6"/>
       <c r="G56" s="8" t="str">
         <f>IF(F56&lt;&gt;"",VLOOKUP(F56,localização[],3,FALSE),"")</f>
@@ -2705,7 +2837,10 @@
       <c r="B57" s="6"/>
       <c r="C57" s="7"/>
       <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
+      <c r="E57" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F57" s="6"/>
       <c r="G57" s="8" t="str">
         <f>IF(F57&lt;&gt;"",VLOOKUP(F57,localização[],3,FALSE),"")</f>
@@ -2717,7 +2852,10 @@
       <c r="B58" s="6"/>
       <c r="C58" s="7"/>
       <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
+      <c r="E58" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F58" s="6"/>
       <c r="G58" s="8" t="str">
         <f>IF(F58&lt;&gt;"",VLOOKUP(F58,localização[],3,FALSE),"")</f>
@@ -2729,7 +2867,10 @@
       <c r="B59" s="6"/>
       <c r="C59" s="7"/>
       <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
+      <c r="E59" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F59" s="6"/>
       <c r="G59" s="8" t="str">
         <f>IF(F59&lt;&gt;"",VLOOKUP(F59,localização[],3,FALSE),"")</f>
@@ -2741,7 +2882,10 @@
       <c r="B60" s="6"/>
       <c r="C60" s="7"/>
       <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+      <c r="E60" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F60" s="6"/>
       <c r="G60" s="8" t="str">
         <f>IF(F60&lt;&gt;"",VLOOKUP(F60,localização[],3,FALSE),"")</f>
@@ -2753,7 +2897,10 @@
       <c r="B61" s="6"/>
       <c r="C61" s="7"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
+      <c r="E61" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F61" s="6"/>
       <c r="G61" s="8" t="str">
         <f>IF(F61&lt;&gt;"",VLOOKUP(F61,localização[],3,FALSE),"")</f>
@@ -2765,7 +2912,10 @@
       <c r="B62" s="6"/>
       <c r="C62" s="7"/>
       <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
+      <c r="E62" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F62" s="6"/>
       <c r="G62" s="8" t="str">
         <f>IF(F62&lt;&gt;"",VLOOKUP(F62,localização[],3,FALSE),"")</f>
@@ -2777,7 +2927,10 @@
       <c r="B63" s="6"/>
       <c r="C63" s="7"/>
       <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
+      <c r="E63" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F63" s="6"/>
       <c r="G63" s="8" t="str">
         <f>IF(F63&lt;&gt;"",VLOOKUP(F63,localização[],3,FALSE),"")</f>
@@ -2789,7 +2942,10 @@
       <c r="B64" s="6"/>
       <c r="C64" s="7"/>
       <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
+      <c r="E64" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F64" s="6"/>
       <c r="G64" s="8" t="str">
         <f>IF(F64&lt;&gt;"",VLOOKUP(F64,localização[],3,FALSE),"")</f>
@@ -2801,7 +2957,10 @@
       <c r="B65" s="6"/>
       <c r="C65" s="7"/>
       <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
+      <c r="E65" s="45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="F65" s="6"/>
       <c r="G65" s="8" t="str">
         <f>IF(F65&lt;&gt;"",VLOOKUP(F65,localização[],3,FALSE),"")</f>
@@ -2813,7 +2972,10 @@
       <c r="B66" s="6"/>
       <c r="C66" s="7"/>
       <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
+      <c r="E66" s="45" t="str">
+        <f t="shared" ref="E66:E99" si="1">IF(A66&lt;&gt;"","FELIPE PINTO DE SOUZA","")</f>
+        <v/>
+      </c>
       <c r="F66" s="6"/>
       <c r="G66" s="8" t="str">
         <f>IF(F66&lt;&gt;"",VLOOKUP(F66,localização[],3,FALSE),"")</f>
@@ -2825,7 +2987,10 @@
       <c r="B67" s="6"/>
       <c r="C67" s="7"/>
       <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+      <c r="E67" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F67" s="6"/>
       <c r="G67" s="8" t="str">
         <f>IF(F67&lt;&gt;"",VLOOKUP(F67,localização[],3,FALSE),"")</f>
@@ -2837,7 +3002,10 @@
       <c r="B68" s="6"/>
       <c r="C68" s="7"/>
       <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
+      <c r="E68" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F68" s="6"/>
       <c r="G68" s="8" t="str">
         <f>IF(F68&lt;&gt;"",VLOOKUP(F68,localização[],3,FALSE),"")</f>
@@ -2849,7 +3017,10 @@
       <c r="B69" s="6"/>
       <c r="C69" s="7"/>
       <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
+      <c r="E69" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F69" s="6"/>
       <c r="G69" s="8" t="str">
         <f>IF(F69&lt;&gt;"",VLOOKUP(F69,localização[],3,FALSE),"")</f>
@@ -2861,7 +3032,10 @@
       <c r="B70" s="6"/>
       <c r="C70" s="7"/>
       <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
+      <c r="E70" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F70" s="6"/>
       <c r="G70" s="8" t="str">
         <f>IF(F70&lt;&gt;"",VLOOKUP(F70,localização[],3,FALSE),"")</f>
@@ -2873,7 +3047,10 @@
       <c r="B71" s="6"/>
       <c r="C71" s="7"/>
       <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
+      <c r="E71" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F71" s="6"/>
       <c r="G71" s="8" t="str">
         <f>IF(F71&lt;&gt;"",VLOOKUP(F71,localização[],3,FALSE),"")</f>
@@ -2885,7 +3062,10 @@
       <c r="B72" s="6"/>
       <c r="C72" s="7"/>
       <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
+      <c r="E72" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F72" s="6"/>
       <c r="G72" s="8" t="str">
         <f>IF(F72&lt;&gt;"",VLOOKUP(F72,localização[],3,FALSE),"")</f>
@@ -2897,7 +3077,10 @@
       <c r="B73" s="6"/>
       <c r="C73" s="7"/>
       <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+      <c r="E73" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F73" s="6"/>
       <c r="G73" s="8" t="str">
         <f>IF(F73&lt;&gt;"",VLOOKUP(F73,localização[],3,FALSE),"")</f>
@@ -2909,7 +3092,10 @@
       <c r="B74" s="6"/>
       <c r="C74" s="7"/>
       <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
+      <c r="E74" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F74" s="6"/>
       <c r="G74" s="8" t="str">
         <f>IF(F74&lt;&gt;"",VLOOKUP(F74,localização[],3,FALSE),"")</f>
@@ -2921,7 +3107,10 @@
       <c r="B75" s="6"/>
       <c r="C75" s="7"/>
       <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
+      <c r="E75" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F75" s="6"/>
       <c r="G75" s="8" t="str">
         <f>IF(F75&lt;&gt;"",VLOOKUP(F75,localização[],3,FALSE),"")</f>
@@ -2933,7 +3122,10 @@
       <c r="B76" s="6"/>
       <c r="C76" s="7"/>
       <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
+      <c r="E76" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F76" s="6"/>
       <c r="G76" s="8" t="str">
         <f>IF(F76&lt;&gt;"",VLOOKUP(F76,localização[],3,FALSE),"")</f>
@@ -2945,7 +3137,10 @@
       <c r="B77" s="6"/>
       <c r="C77" s="7"/>
       <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
+      <c r="E77" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F77" s="6"/>
       <c r="G77" s="8" t="str">
         <f>IF(F77&lt;&gt;"",VLOOKUP(F77,localização[],3,FALSE),"")</f>
@@ -2957,7 +3152,10 @@
       <c r="B78" s="6"/>
       <c r="C78" s="7"/>
       <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
+      <c r="E78" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F78" s="6"/>
       <c r="G78" s="8" t="str">
         <f>IF(F78&lt;&gt;"",VLOOKUP(F78,localização[],3,FALSE),"")</f>
@@ -2969,7 +3167,10 @@
       <c r="B79" s="6"/>
       <c r="C79" s="7"/>
       <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
+      <c r="E79" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F79" s="6"/>
       <c r="G79" s="8" t="str">
         <f>IF(F79&lt;&gt;"",VLOOKUP(F79,localização[],3,FALSE),"")</f>
@@ -2981,7 +3182,10 @@
       <c r="B80" s="6"/>
       <c r="C80" s="7"/>
       <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
+      <c r="E80" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F80" s="6"/>
       <c r="G80" s="8" t="str">
         <f>IF(F80&lt;&gt;"",VLOOKUP(F80,localização[],3,FALSE),"")</f>
@@ -2993,7 +3197,10 @@
       <c r="B81" s="6"/>
       <c r="C81" s="7"/>
       <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
+      <c r="E81" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F81" s="6"/>
       <c r="G81" s="8" t="str">
         <f>IF(F81&lt;&gt;"",VLOOKUP(F81,localização[],3,FALSE),"")</f>
@@ -3005,7 +3212,10 @@
       <c r="B82" s="6"/>
       <c r="C82" s="7"/>
       <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
+      <c r="E82" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F82" s="6"/>
       <c r="G82" s="8" t="str">
         <f>IF(F82&lt;&gt;"",VLOOKUP(F82,localização[],3,FALSE),"")</f>
@@ -3017,7 +3227,10 @@
       <c r="B83" s="6"/>
       <c r="C83" s="7"/>
       <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
+      <c r="E83" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F83" s="6"/>
       <c r="G83" s="8" t="str">
         <f>IF(F83&lt;&gt;"",VLOOKUP(F83,localização[],3,FALSE),"")</f>
@@ -3029,7 +3242,10 @@
       <c r="B84" s="6"/>
       <c r="C84" s="7"/>
       <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
+      <c r="E84" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F84" s="6"/>
       <c r="G84" s="8" t="str">
         <f>IF(F84&lt;&gt;"",VLOOKUP(F84,localização[],3,FALSE),"")</f>
@@ -3041,7 +3257,10 @@
       <c r="B85" s="6"/>
       <c r="C85" s="7"/>
       <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
+      <c r="E85" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F85" s="6"/>
       <c r="G85" s="8" t="str">
         <f>IF(F85&lt;&gt;"",VLOOKUP(F85,localização[],3,FALSE),"")</f>
@@ -3053,7 +3272,10 @@
       <c r="B86" s="6"/>
       <c r="C86" s="7"/>
       <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
+      <c r="E86" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F86" s="6"/>
       <c r="G86" s="8" t="str">
         <f>IF(F86&lt;&gt;"",VLOOKUP(F86,localização[],3,FALSE),"")</f>
@@ -3065,7 +3287,10 @@
       <c r="B87" s="6"/>
       <c r="C87" s="7"/>
       <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
+      <c r="E87" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F87" s="6"/>
       <c r="G87" s="8" t="str">
         <f>IF(F87&lt;&gt;"",VLOOKUP(F87,localização[],3,FALSE),"")</f>
@@ -3077,7 +3302,10 @@
       <c r="B88" s="6"/>
       <c r="C88" s="7"/>
       <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
+      <c r="E88" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F88" s="6"/>
       <c r="G88" s="8" t="str">
         <f>IF(F88&lt;&gt;"",VLOOKUP(F88,localização[],3,FALSE),"")</f>
@@ -3089,7 +3317,10 @@
       <c r="B89" s="6"/>
       <c r="C89" s="7"/>
       <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
+      <c r="E89" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F89" s="6"/>
       <c r="G89" s="8" t="str">
         <f>IF(F89&lt;&gt;"",VLOOKUP(F89,localização[],3,FALSE),"")</f>
@@ -3101,7 +3332,10 @@
       <c r="B90" s="6"/>
       <c r="C90" s="7"/>
       <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
+      <c r="E90" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F90" s="6"/>
       <c r="G90" s="8" t="str">
         <f>IF(F90&lt;&gt;"",VLOOKUP(F90,localização[],3,FALSE),"")</f>
@@ -3113,7 +3347,10 @@
       <c r="B91" s="6"/>
       <c r="C91" s="7"/>
       <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
+      <c r="E91" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F91" s="6"/>
       <c r="G91" s="8" t="str">
         <f>IF(F91&lt;&gt;"",VLOOKUP(F91,localização[],3,FALSE),"")</f>
@@ -3125,7 +3362,10 @@
       <c r="B92" s="6"/>
       <c r="C92" s="7"/>
       <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
+      <c r="E92" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F92" s="6"/>
       <c r="G92" s="8" t="str">
         <f>IF(F92&lt;&gt;"",VLOOKUP(F92,localização[],3,FALSE),"")</f>
@@ -3137,7 +3377,10 @@
       <c r="B93" s="6"/>
       <c r="C93" s="7"/>
       <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+      <c r="E93" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F93" s="6"/>
       <c r="G93" s="8" t="str">
         <f>IF(F93&lt;&gt;"",VLOOKUP(F93,localização[],3,FALSE),"")</f>
@@ -3149,7 +3392,10 @@
       <c r="B94" s="6"/>
       <c r="C94" s="7"/>
       <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
+      <c r="E94" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F94" s="6"/>
       <c r="G94" s="8" t="str">
         <f>IF(F94&lt;&gt;"",VLOOKUP(F94,localização[],3,FALSE),"")</f>
@@ -3161,7 +3407,10 @@
       <c r="B95" s="6"/>
       <c r="C95" s="7"/>
       <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
+      <c r="E95" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F95" s="6"/>
       <c r="G95" s="8" t="str">
         <f>IF(F95&lt;&gt;"",VLOOKUP(F95,localização[],3,FALSE),"")</f>
@@ -3173,7 +3422,10 @@
       <c r="B96" s="6"/>
       <c r="C96" s="7"/>
       <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
+      <c r="E96" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F96" s="6"/>
       <c r="G96" s="8" t="str">
         <f>IF(F96&lt;&gt;"",VLOOKUP(F96,localização[],3,FALSE),"")</f>
@@ -3185,7 +3437,10 @@
       <c r="B97" s="6"/>
       <c r="C97" s="7"/>
       <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
+      <c r="E97" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F97" s="6"/>
       <c r="G97" s="8" t="str">
         <f>IF(F97&lt;&gt;"",VLOOKUP(F97,localização[],3,FALSE),"")</f>
@@ -3197,7 +3452,10 @@
       <c r="B98" s="6"/>
       <c r="C98" s="7"/>
       <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
+      <c r="E98" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F98" s="6"/>
       <c r="G98" s="8" t="str">
         <f>IF(F98&lt;&gt;"",VLOOKUP(F98,localização[],3,FALSE),"")</f>
@@ -3209,22 +3467,13 @@
       <c r="B99" s="6"/>
       <c r="C99" s="7"/>
       <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
+      <c r="E99" s="45" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
       <c r="F99" s="6"/>
       <c r="G99" s="8" t="str">
         <f>IF(F99&lt;&gt;"",VLOOKUP(F99,localização[],3,FALSE),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="5"/>
-      <c r="B100" s="6"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="6"/>
-      <c r="G100" s="8" t="str">
-        <f>IF(F100&lt;&gt;"",VLOOKUP(F100,localização[],3,FALSE),"")</f>
         <v/>
       </c>
     </row>
@@ -3232,33 +3481,30 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E2 E12:E99 E4:E10" unlockedFormula="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A49C1178-713D-4ED8-8186-C11DFDB35620}">
-          <x14:formula1>
-            <xm:f>ATRIBUIDO!$A$2:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E100</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C9A6595-EDA6-4FDD-BEE4-CFDBA6C2442B}">
           <x14:formula1>
-            <xm:f>TITULO!$A$2:$A$48</xm:f>
+            <xm:f>TITULO!$A$2:$A$51</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A100</xm:sqref>
+          <xm:sqref>A2:A99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{44535B38-A774-43E8-972F-F53B5F161002}">
           <x14:formula1>
             <xm:f>CATEGORIA!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D100</xm:sqref>
+          <xm:sqref>D2:D99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{89F359FB-FF17-4F39-B13E-63860C6FF08E}">
           <x14:formula1>
-            <xm:f>LOCALIZAÇÃO!$A$2:$A$100</xm:f>
+            <xm:f>LOCALIZAÇÃO!$A$2:$A$102</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F100</xm:sqref>
+          <xm:sqref>F2:F99</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3268,10 +3514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5070748A-A2E0-4296-9F3D-CFF9CF15F663}">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,242 +3527,257 @@
   <sheetData>
     <row r="1" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>62</v>
+      <c r="A3" s="16" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>64</v>
+      <c r="A5" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>66</v>
+      <c r="A7" s="16" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>68</v>
+      <c r="A9" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>69</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>241</v>
+      <c r="A11" s="16" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>285</v>
+      <c r="A12" s="16" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="34" t="s">
-        <v>70</v>
+      <c r="A13" s="16" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
-        <v>71</v>
+      <c r="A14" s="16" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="34" t="s">
-        <v>140</v>
+      <c r="A15" s="33" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>72</v>
+      <c r="A16" s="16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="34" t="s">
-        <v>73</v>
+      <c r="A17" s="33" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="17" t="s">
-        <v>74</v>
+      <c r="A18" s="16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="34" t="s">
-        <v>75</v>
+      <c r="A19" s="33" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="17" t="s">
-        <v>76</v>
+      <c r="A20" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="34" t="s">
-        <v>77</v>
+      <c r="A21" s="33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="17" t="s">
-        <v>78</v>
+      <c r="A22" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>79</v>
+      <c r="A23" s="33" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A27" s="33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="34" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="34" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="34" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="34" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="34" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="34" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="34" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="17" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="35" t="s">
-        <v>100</v>
+    <row r="48" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="34" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -3529,7 +3790,7 @@
   <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3539,17 +3800,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>145</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>146</v>
+      <c r="A3" s="16" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -3558,98 +3819,98 @@
       </c>
     </row>
     <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>147</v>
+      <c r="A5" s="16" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>149</v>
+      <c r="A7" s="16" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>150</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>151</v>
+      <c r="A9" s="16" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>152</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>155</v>
+      <c r="A11" s="16" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>157</v>
+      <c r="A13" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>158</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>159</v>
+      <c r="A15" s="16" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>160</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>161</v>
+      <c r="A17" s="16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>162</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
-        <v>163</v>
+      <c r="A19" s="16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>164</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>165</v>
+      <c r="A21" s="16" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>166</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
-        <v>167</v>
+      <c r="A23" s="16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -3690,7 +3951,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -3699,58 +3960,58 @@
       </c>
     </row>
     <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
-        <v>128</v>
+      <c r="A3" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>130</v>
+      <c r="A5" s="16" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>132</v>
+      <c r="A7" s="16" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>134</v>
+      <c r="A9" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>135</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>136</v>
+      <c r="A11" s="16" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>137</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>138</v>
+      <c r="A13" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
@@ -3844,10 +4105,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377FF143-C3F8-4C93-9956-8A72982D22B7}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3864,1047 +4125,1065 @@
       <c r="B1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="38" t="s">
-        <v>24</v>
+      <c r="C1" s="37" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="40" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="40" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="B7" s="19"/>
+      <c r="C7" s="40" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="43" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="43" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="19"/>
+      <c r="C10" s="40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="40" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="40" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="40" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="40" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="43" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="43" t="s">
+        <v>202</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="43" t="s">
+        <v>203</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="40" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="43" t="s">
+        <v>205</v>
+      </c>
+      <c r="B20" s="19"/>
+      <c r="C20" s="40" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="43" t="s">
+        <v>206</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="40" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="40" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="43" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="40" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="43" t="s">
+        <v>209</v>
+      </c>
+      <c r="B24" s="19"/>
+      <c r="C24" s="40" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="43" t="s">
+        <v>292</v>
+      </c>
+      <c r="B25" s="19"/>
+      <c r="C25" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="B26" s="19"/>
+      <c r="C26" s="40" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="40" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="40" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A30" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A36" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A39" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="39" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="39" t="s">
+    </row>
+    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="39" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="40" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="39" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="40" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="39" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A55" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="39" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A58" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="39" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A60" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="B60" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="39" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A62" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="40" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A63" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="39" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A64" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="40" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C65" s="39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A66" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="40" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A67" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" s="39" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A68" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" s="39" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" s="40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" s="39" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" s="40" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="39" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A75" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" s="39" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A76" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" s="40" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" s="39" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A78" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="40" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A79" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="39" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A80" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="40" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A81" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C81" s="39" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A82" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C82" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A83" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="39" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A84" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="40" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="39" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+    <row r="86" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A86" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B86" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" s="39" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A88" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C88" s="40" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A89" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C89" s="39" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A90" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C90" s="40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A91" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C91" s="39" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A92" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C92" s="40" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="39" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C94" s="40" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A95" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="39" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A96" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B96" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="40" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A97" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B97" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" s="39" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="B98" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" s="40" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99" s="39" t="s">
         <v>243</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="39" t="s">
+    </row>
+    <row r="100" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A100" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100" s="40" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="44" t="s">
-        <v>265</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="41" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
-        <v>245</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="41" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
-        <v>266</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="41" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="44" t="s">
-        <v>267</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="41" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="41" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
-        <v>269</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="41" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="44" t="s">
-        <v>270</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="41" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="44" t="s">
-        <v>271</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="41" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="44" t="s">
-        <v>272</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="41" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="44" t="s">
-        <v>273</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="41" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="44" t="s">
-        <v>274</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="41" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="44" t="s">
-        <v>275</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="44" t="s">
-        <v>276</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="41" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="41" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="44" t="s">
-        <v>278</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="41" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="44" t="s">
-        <v>279</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="41" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="44" t="s">
-        <v>280</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="41" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="44" t="s">
-        <v>281</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="41" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="44" t="s">
-        <v>282</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="41" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="44" t="s">
-        <v>283</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="41" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="44" t="s">
-        <v>284</v>
-      </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="41" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="44" t="s">
-        <v>287</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="41" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="B27" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="40" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="B32" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="40" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="B34" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="41" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="37" t="s">
+    <row r="101" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="B36" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="36" t="s">
+      <c r="B101" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" s="39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A102" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
-        <v>180</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="B40" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="41" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41" s="40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="B45" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C48" s="41" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="B49" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C50" s="41" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="37" t="s">
-        <v>194</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C52" s="41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="B53" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C53" s="40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C56" s="41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="36" t="s">
-        <v>199</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="40" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="41" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="36" t="s">
-        <v>201</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C59" s="40" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="B60" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C60" s="41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="B61" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="C61" s="40" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B62" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C62" s="41" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C63" s="40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="37" t="s">
-        <v>204</v>
-      </c>
-      <c r="B64" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C64" s="41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="B65" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C65" s="40" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="B66" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C66" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="36" t="s">
-        <v>207</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C67" s="40" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="B68" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C68" s="41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C69" s="40" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C70" s="41" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="36" t="s">
-        <v>211</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C71" s="40" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="B72" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C72" s="41" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="36" t="s">
-        <v>213</v>
-      </c>
-      <c r="B73" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C73" s="40" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="B74" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C74" s="41" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="B75" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C75" s="40" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="B76" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76" s="41" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="36" t="s">
-        <v>217</v>
-      </c>
-      <c r="B77" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C77" s="40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="B78" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C78" s="41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C79" s="40" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C81" s="40" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="37" t="s">
-        <v>222</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C82" s="41" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="36" t="s">
-        <v>223</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" s="40" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="B84" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C84" s="41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="B85" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85" s="40" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="B86" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C86" s="41" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="B87" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C87" s="40" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A88" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C88" s="41" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A89" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C89" s="40" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A90" s="37" t="s">
-        <v>230</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C90" s="41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A91" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" s="40" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="B92" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C92" s="41" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="B93" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C93" s="40" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A94" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="B94" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C94" s="41" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A95" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B95" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C95" s="40" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="37" t="s">
+      <c r="B102" s="41"/>
+      <c r="C102" s="42" t="s">
         <v>236</v>
-      </c>
-      <c r="B96" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C96" s="41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A97" s="36" t="s">
-        <v>237</v>
-      </c>
-      <c r="B97" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C97" s="40" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A98" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="B98" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C98" s="41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="36" t="s">
-        <v>239</v>
-      </c>
-      <c r="B99" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C99" s="40" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A100" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="B100" s="42"/>
-      <c r="C100" s="43" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>